<commit_message>
feat: Add solution saving and loading functionality, Gurobi license example, and update solver logic, results, and project configuration.
</commit_message>
<xml_diff>
--- a/results/solutions/experiment_results.xlsx
+++ b/results/solutions/experiment_results.xlsx
@@ -495,7 +495,7 @@
         <v>734700</v>
       </c>
       <c r="D2" t="n">
-        <v>6.986764192581177</v>
+        <v>7.002241134643555</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
@@ -524,7 +524,7 @@
         <v>652185</v>
       </c>
       <c r="D3" t="n">
-        <v>6.305203914642334</v>
+        <v>6.158377170562744</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
@@ -553,7 +553,7 @@
         <v>537820</v>
       </c>
       <c r="D4" t="n">
-        <v>6.504022836685181</v>
+        <v>6.489912748336792</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">

</xml_diff>